<commit_message>
This version contains the UpdateByTag operation
</commit_message>
<xml_diff>
--- a/ConsoleApp1/AzureDevOpsImport.xlsx
+++ b/ConsoleApp1/AzureDevOpsImport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\ConsoleApp1\ConsoleApp1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B036D5-AC38-4436-817C-AEDBFB8BFA03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97AB7140-A716-4B0F-A36D-3A257DB3ABE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="732" yWindow="624" windowWidth="20100" windowHeight="11616" xr2:uid="{DC355886-F2A8-4F83-B9C9-445C553A4E0B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="54">
   <si>
     <t>Server Location</t>
   </si>
@@ -348,7 +348,31 @@
     <t>Iteration ID</t>
   </si>
   <si>
-    <t>ddd</t>
+    <t>UpdateByTag</t>
+  </si>
+  <si>
+    <t>Tag2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brilliant Bulk Update </t>
+  </si>
+  <si>
+    <t>Bug</t>
+  </si>
+  <si>
+    <t>Update Operation</t>
+  </si>
+  <si>
+    <t>UpdateByTag Operation</t>
+  </si>
+  <si>
+    <t>New Title to Be added to all Bugs with this tag</t>
+  </si>
+  <si>
+    <t>New Desc.</t>
+  </si>
+  <si>
+    <t>Tag to search</t>
   </si>
 </sst>
 </file>
@@ -766,9 +790,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5DB5797-8B65-4B31-ADFF-F8F00341DC48}">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -860,16 +884,16 @@
     </row>
     <row r="5" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G5" s="1">
-        <v>53</v>
+      <c r="D5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -966,181 +990,217 @@
       <c r="A24" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" ht="21.3" x14ac:dyDescent="0.85">
+      <c r="B24" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="21.3" x14ac:dyDescent="0.85">
+      <c r="A27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="21.3" x14ac:dyDescent="0.85">
-      <c r="A26" t="s">
-        <v>17</v>
-      </c>
-      <c r="B26" s="3" t="s">
+    <row r="28" spans="1:11" ht="21.3" x14ac:dyDescent="0.85">
+      <c r="A28" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" t="s">
-        <v>17</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E27" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G27" t="s">
-        <v>3</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I27" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" t="s">
-        <v>17</v>
-      </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>17</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>12</v>
+        <v>0</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>14</v>
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>10</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="G29" t="s">
+        <v>3</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I29" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J29" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K29" s="4"/>
+        <v>34</v>
+      </c>
+      <c r="I29" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>17</v>
       </c>
-      <c r="B30" t="s">
-        <v>16</v>
-      </c>
-      <c r="C30" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" t="s">
-        <v>29</v>
-      </c>
-      <c r="E30" t="s">
-        <v>28</v>
-      </c>
-      <c r="F30">
-        <v>2</v>
-      </c>
-      <c r="G30">
-        <v>1</v>
-      </c>
-      <c r="J30" t="s">
-        <v>33</v>
-      </c>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="F30" s="4"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>17</v>
       </c>
-      <c r="B31" t="s">
-        <v>16</v>
-      </c>
-      <c r="C31" t="s">
-        <v>11</v>
-      </c>
-      <c r="D31" t="s">
-        <v>30</v>
-      </c>
-      <c r="E31" t="s">
-        <v>28</v>
-      </c>
-      <c r="F31">
-        <v>2</v>
-      </c>
-      <c r="G31">
-        <v>1</v>
-      </c>
-      <c r="H31">
-        <v>23</v>
-      </c>
+      <c r="B31" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K31" s="4"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>17</v>
       </c>
       <c r="B32" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" t="s">
+        <v>29</v>
+      </c>
+      <c r="E32" t="s">
+        <v>28</v>
+      </c>
+      <c r="F32">
+        <v>2</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="J32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" t="s">
+        <v>30</v>
+      </c>
+      <c r="E33" t="s">
+        <v>28</v>
+      </c>
+      <c r="F33">
+        <v>2</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" t="s">
         <v>27</v>
       </c>
-      <c r="I32">
+      <c r="I34">
         <v>123</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" t="s">
-        <v>17</v>
-      </c>
-      <c r="B33" t="s">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" t="s">
         <v>26</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C35" t="s">
         <v>31</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D35" t="s">
         <v>32</v>
       </c>
-      <c r="G33">
+      <c r="G35">
         <v>2</v>
       </c>
-      <c r="I33">
+      <c r="I35">
         <v>123</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B36" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" t="s">
+        <v>48</v>
+      </c>
+      <c r="D36" t="s">
+        <v>51</v>
+      </c>
+      <c r="E36" t="s">
+        <v>52</v>
+      </c>
+      <c r="J36" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection insertRows="0" selectLockedCells="1"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{257D91CD-44B5-4BBC-98E7-5F1E1703D6FC}"/>
-    <hyperlink ref="C27" r:id="rId2" xr:uid="{0BB6E2F2-49A7-402A-A110-6A5EC9B40CB6}"/>
+    <hyperlink ref="C29" r:id="rId2" xr:uid="{0BB6E2F2-49A7-402A-A110-6A5EC9B40CB6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>

</xml_diff>